<commit_message>
Implemented LDDT() class in lddt.py, pylddt_foldmason.py passed first test
</commit_message>
<xml_diff>
--- a/results/pylddt_results.xlsx
+++ b/results/pylddt_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\pylddt\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4976D66-D762-43EA-9F17-7176B9F6140E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29CCB62-7577-42D0-9A80-E9F3FEB9CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9735" yWindow="4050" windowWidth="23055" windowHeight="14850" xr2:uid="{DAEDAB50-C799-4EBA-AB77-2A1974DF6EA3}"/>
+    <workbookView xWindow="7755" yWindow="4185" windowWidth="23055" windowHeight="14850" xr2:uid="{DAEDAB50-C799-4EBA-AB77-2A1974DF6EA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
-  <si>
-    <t>Set</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t xml:space="preserve"> 1aab_1j46</t>
   </si>
@@ -59,13 +56,10 @@
     <t>OS</t>
   </si>
   <si>
-    <t>pylddt(or)</t>
-  </si>
-  <si>
-    <t>pylddt(and)</t>
-  </si>
-  <si>
-    <t>pfm</t>
+    <t>pylddt</t>
+  </si>
+  <si>
+    <t>set</t>
   </si>
 </sst>
 </file>
@@ -75,8 +69,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -104,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -116,6 +118,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -452,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEBABDE-16C4-4BD2-AA78-1E88DEC6E456}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -461,37 +469,30 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="4" width="14.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="18.140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3"/>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>12</v>
       </c>
@@ -499,23 +500,17 @@
         <v>0.50280000000000002</v>
       </c>
       <c r="C2" s="4">
-        <v>0.52639999999999998</v>
+        <v>0.48970000000000002</v>
       </c>
       <c r="D2" s="4">
-        <v>0.4647</v>
+        <v>0.489701</v>
       </c>
       <c r="E2" s="4">
-        <v>0.489701</v>
-      </c>
-      <c r="F2" s="4">
         <v>0.49490000000000001</v>
       </c>
-      <c r="G2" s="2">
-        <v>0.48970000000000002</v>
-      </c>
-      <c r="I2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>21</v>
       </c>
@@ -523,23 +518,17 @@
         <v>0.50629999999999997</v>
       </c>
       <c r="C3" s="4">
-        <v>0.52639999999999998</v>
+        <v>0.49330000000000002</v>
       </c>
       <c r="D3" s="4">
-        <v>0.4647</v>
+        <v>0.489701</v>
       </c>
       <c r="E3" s="4">
-        <v>0.489701</v>
-      </c>
-      <c r="F3" s="4">
         <v>0.48759999999999998</v>
       </c>
-      <c r="G3" s="2">
-        <v>0.49330000000000002</v>
-      </c>
-      <c r="I3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45</v>
       </c>
@@ -547,23 +536,17 @@
         <v>0.63060000000000005</v>
       </c>
       <c r="C4" s="4">
-        <v>0.63400000000000001</v>
+        <v>0.62060000000000004</v>
       </c>
       <c r="D4" s="4">
-        <v>0.59950000000000003</v>
+        <v>0.62055000000000005</v>
       </c>
       <c r="E4" s="4">
-        <v>0.62055000000000005</v>
-      </c>
-      <c r="F4" s="4">
         <v>0.60950000000000004</v>
       </c>
-      <c r="G4" s="2">
-        <v>0.62060000000000004</v>
-      </c>
-      <c r="I4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>54</v>
       </c>
@@ -571,71 +554,54 @@
         <v>0.61680000000000001</v>
       </c>
       <c r="C5" s="4">
-        <v>0.63400000000000001</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="D5" s="4">
-        <v>0.59950000000000003</v>
+        <v>0.62055000000000005</v>
       </c>
       <c r="E5" s="4">
-        <v>0.62055000000000005</v>
-      </c>
-      <c r="F5" s="4">
         <v>0.62109999999999999</v>
       </c>
-      <c r="G5" s="2">
-        <v>0.60699999999999998</v>
-      </c>
-      <c r="I5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.54157100000000002</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.78839999999999999</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.72309999999999997</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.54157100000000002</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.57120000000000004</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4">
-        <v>0.78249999999999997</v>
+        <v>0.62570000000000003</v>
       </c>
       <c r="D7" s="4">
-        <v>0.70309999999999995</v>
-      </c>
-      <c r="E7" s="4">
         <v>0.61303099999999999</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.62570000000000003</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>